<commit_message>
lagt til ny toggle button komponent + def + off rating ESF
</commit_message>
<xml_diff>
--- a/stored_data/eliteserien/2023/fixture_data/Eliteserien_fixtures.xlsx
+++ b/stored_data/eliteserien/2023/fixture_data/Eliteserien_fixtures.xlsx
@@ -587,7 +587,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -749,11 +749,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1035,6 +1065,24 @@
     <xf numFmtId="0" fontId="2" fillId="29" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1253,7 +1301,7 @@
   <dimension ref="A1:S982"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="B3" sqref="B3:K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1349,34 +1397,34 @@
       <c r="A3" s="86" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="102" t="s">
+      <c r="B3" s="111" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="103" t="s">
+      <c r="C3" s="112" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="104" t="s">
+      <c r="D3" s="113" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="105" t="s">
+      <c r="E3" s="114" t="s">
         <v>71</v>
       </c>
-      <c r="F3" s="106" t="s">
+      <c r="F3" s="115" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="106" t="s">
+      <c r="G3" s="115" t="s">
         <v>50</v>
       </c>
-      <c r="H3" s="104" t="s">
+      <c r="H3" s="113" t="s">
         <v>29</v>
       </c>
-      <c r="I3" s="104" t="s">
+      <c r="I3" s="113" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="103" t="s">
+      <c r="J3" s="112" t="s">
         <v>52</v>
       </c>
-      <c r="K3" s="106" t="s">
+      <c r="K3" s="115" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1405,10 +1453,10 @@
       <c r="H4" s="109" t="s">
         <v>33</v>
       </c>
-      <c r="I4" s="109" t="s">
+      <c r="I4" s="108" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="109" t="s">
+      <c r="J4" s="108" t="s">
         <v>13</v>
       </c>
       <c r="K4" s="108" t="s">
@@ -1457,7 +1505,7 @@
       <c r="B6" s="102" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="106" t="s">
+      <c r="C6" s="103" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="106" t="s">
@@ -1475,7 +1523,7 @@
       <c r="H6" s="103" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="106" t="s">
+      <c r="I6" s="103" t="s">
         <v>37</v>
       </c>
       <c r="J6" s="104" t="s">
@@ -1489,10 +1537,10 @@
       <c r="A7" s="90" t="s">
         <v>58</v>
       </c>
-      <c r="B7" s="110" t="s">
+      <c r="B7" s="116" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="106" t="s">
+      <c r="C7" s="109" t="s">
         <v>25</v>
       </c>
       <c r="D7" s="106" t="s">
@@ -1542,10 +1590,10 @@
       <c r="G8" s="106" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="106" t="s">
+      <c r="H8" s="109" t="s">
         <v>22</v>
       </c>
-      <c r="I8" s="106" t="s">
+      <c r="I8" s="109" t="s">
         <v>23</v>
       </c>
       <c r="J8" s="108" t="s">
@@ -1676,7 +1724,7 @@
       <c r="E12" s="106" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="103" t="s">
+      <c r="F12" s="104" t="s">
         <v>53</v>
       </c>
       <c r="G12" s="106" t="s">
@@ -1717,7 +1765,7 @@
       <c r="G13" s="106" t="s">
         <v>52</v>
       </c>
-      <c r="H13" s="106" t="s">
+      <c r="H13" s="103" t="s">
         <v>38</v>
       </c>
       <c r="I13" s="108" t="s">
@@ -1860,7 +1908,7 @@
       <c r="H17" s="106" t="s">
         <v>16</v>
       </c>
-      <c r="I17" s="103" t="s">
+      <c r="I17" s="104" t="s">
         <v>8</v>
       </c>
       <c r="J17" s="103" t="s">
@@ -1898,7 +1946,7 @@
       <c r="I18" s="106" t="s">
         <v>50</v>
       </c>
-      <c r="J18" s="103" t="s">
+      <c r="J18" s="108" t="s">
         <v>12</v>
       </c>
       <c r="K18" s="109" t="s">

</xml_diff>